<commit_message>
removed 1 qrest sop
the level 1 sop for qrest needs to be edited to include only internal-to-monitoring-network checks, leaving the level 2 review to include outside data from downwind sites
</commit_message>
<xml_diff>
--- a/hosted_files/QREST/QREST-Level 2 Data Review.xlsx
+++ b/hosted_files/QREST/QREST-Level 2 Data Review.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melinda\Dropbox (NAU Research)\QREST-Team\QREST-training\SOPs\Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melinda\Documents\GitHub\tamscenter.github.io\hosted_files\QREST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AF43C1-8C8D-47E5-A721-F0548EFD08CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BF1B752-6DBA-4F6D-9A62-8D5EB8FCC9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-50" windowWidth="19420" windowHeight="10560" xr2:uid="{7715871D-8683-4309-BD27-314EA3A9CF8F}"/>
+    <workbookView xWindow="19090" yWindow="-1850" windowWidth="19420" windowHeight="10560" xr2:uid="{7715871D-8683-4309-BD27-314EA3A9CF8F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Level1Review" sheetId="1" r:id="rId1"/>
+    <sheet name="Level2Review" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
     <sheet name="ColorsInDataReviewPanels" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -863,16 +863,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -889,6 +886,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -901,8 +901,8 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -5527,8 +5527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CD1C20-C544-4641-A5D7-3C5C166E6123}">
   <dimension ref="A1:I366"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A265" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5547,7 +5547,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>91</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -5572,14 +5572,14 @@
     </row>
     <row r="2" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="36"/>
+      <c r="B2" s="35"/>
       <c r="G2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="38"/>
+      <c r="I2" s="37"/>
     </row>
     <row r="3" spans="1:9" s="9" customFormat="1" ht="22.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
@@ -5590,8 +5590,8 @@
       <c r="D3" s="40"/>
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
     </row>
     <row r="4" spans="1:9" s="9" customFormat="1" ht="22.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="40"/>
@@ -5601,8 +5601,8 @@
       <c r="E4" s="40"/>
       <c r="F4" s="40"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
     </row>
     <row r="5" spans="1:9" s="9" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="40"/>
@@ -5612,8 +5612,8 @@
       <c r="E5" s="40"/>
       <c r="F5" s="40"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
     </row>
     <row r="6" spans="1:9" s="9" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="40"/>
@@ -5623,8 +5623,8 @@
       <c r="E6" s="40"/>
       <c r="F6" s="40"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
     </row>
     <row r="7" spans="1:9" s="9" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="40"/>
@@ -5634,8 +5634,8 @@
       <c r="E7" s="40"/>
       <c r="F7" s="40"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
     </row>
     <row r="8" spans="1:9" s="9" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="40"/>
@@ -5645,8 +5645,8 @@
       <c r="E8" s="40"/>
       <c r="F8" s="40"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
     </row>
     <row r="9" spans="1:9" s="9" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="40"/>
@@ -5658,10 +5658,10 @@
       <c r="G9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="39"/>
+      <c r="I9" s="38"/>
     </row>
     <row r="10" spans="1:9" s="9" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
@@ -5671,8 +5671,8 @@
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
     </row>
     <row r="11" spans="1:9" s="9" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
@@ -5680,8 +5680,8 @@
         <v>11</v>
       </c>
       <c r="G11" s="14"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
     </row>
     <row r="12" spans="1:9" s="9" customFormat="1" ht="19.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
@@ -5694,7 +5694,7 @@
     </row>
     <row r="13" spans="1:9" s="9" customFormat="1" ht="22.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="39" t="s">
         <v>80</v>
       </c>
       <c r="G13" s="40"/>
@@ -5703,14 +5703,14 @@
     </row>
     <row r="14" spans="1:9" s="9" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
-      <c r="B14" s="32"/>
+      <c r="B14" s="39"/>
       <c r="G14" s="40"/>
       <c r="H14" s="40"/>
       <c r="I14" s="40"/>
     </row>
     <row r="15" spans="1:9" s="9" customFormat="1" ht="25.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
-      <c r="B15" s="32"/>
+      <c r="B15" s="39"/>
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
       <c r="I15" s="40"/>
@@ -5718,59 +5718,59 @@
     <row r="16" spans="1:9" s="9" customFormat="1" ht="25.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
     </row>
     <row r="17" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" s="1"/>
       <c r="D17" s="5"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
     </row>
     <row r="18" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B23" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
@@ -5823,42 +5823,42 @@
       <c r="A56" s="6">
         <v>4</v>
       </c>
-      <c r="B56" s="37" t="s">
+      <c r="B56" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C56" s="37"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="37"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="36"/>
+      <c r="F56" s="36"/>
+      <c r="G56" s="36"/>
+      <c r="H56" s="36"/>
     </row>
     <row r="57" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="37"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="37"/>
-      <c r="H57" s="37"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="36"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B58" s="37"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="37"/>
-      <c r="G58" s="37"/>
-      <c r="H58" s="37"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="36"/>
+      <c r="F58" s="36"/>
+      <c r="G58" s="36"/>
+      <c r="H58" s="36"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="37"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="36"/>
     </row>
     <row r="61" spans="1:9" ht="20" x14ac:dyDescent="0.4">
       <c r="B61"/>
@@ -5867,20 +5867,20 @@
       <c r="B62"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H63" s="34"/>
-      <c r="I63" s="34"/>
+      <c r="H63" s="31"/>
+      <c r="I63" s="31"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H64" s="34"/>
-      <c r="I64" s="34"/>
+      <c r="H64" s="31"/>
+      <c r="I64" s="31"/>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="H65" s="34"/>
-      <c r="I65" s="34"/>
+      <c r="H65" s="31"/>
+      <c r="I65" s="31"/>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="H66" s="34"/>
-      <c r="I66" s="34"/>
+      <c r="H66" s="31"/>
+      <c r="I66" s="31"/>
     </row>
     <row r="68" spans="2:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B68" s="41" t="s">
@@ -5938,45 +5938,45 @@
     </row>
     <row r="74" spans="2:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B74" s="17"/>
-      <c r="C74" s="33" t="s">
+      <c r="C74" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="D74" s="33"/>
-      <c r="E74" s="33"/>
-      <c r="F74" s="33"/>
-      <c r="G74" s="33"/>
-      <c r="H74" s="33"/>
-      <c r="I74" s="33"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="32"/>
+      <c r="F74" s="32"/>
+      <c r="G74" s="32"/>
+      <c r="H74" s="32"/>
+      <c r="I74" s="32"/>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B75" s="17"/>
-      <c r="C75" s="33"/>
-      <c r="D75" s="33"/>
-      <c r="E75" s="33"/>
-      <c r="F75" s="33"/>
-      <c r="G75" s="33"/>
-      <c r="H75" s="33"/>
-      <c r="I75" s="33"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="32"/>
+      <c r="G75" s="32"/>
+      <c r="H75" s="32"/>
+      <c r="I75" s="32"/>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B76" s="27"/>
-      <c r="C76" s="33"/>
-      <c r="D76" s="33"/>
-      <c r="E76" s="33"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="33"/>
-      <c r="H76" s="33"/>
-      <c r="I76" s="33"/>
+      <c r="C76" s="32"/>
+      <c r="D76" s="32"/>
+      <c r="E76" s="32"/>
+      <c r="F76" s="32"/>
+      <c r="G76" s="32"/>
+      <c r="H76" s="32"/>
+      <c r="I76" s="32"/>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B77" s="27"/>
-      <c r="C77" s="33"/>
-      <c r="D77" s="33"/>
-      <c r="E77" s="33"/>
-      <c r="F77" s="33"/>
-      <c r="G77" s="33"/>
-      <c r="H77" s="33"/>
-      <c r="I77" s="33"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="32"/>
+      <c r="E77" s="32"/>
+      <c r="F77" s="32"/>
+      <c r="G77" s="32"/>
+      <c r="H77" s="32"/>
+      <c r="I77" s="32"/>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B78" s="17"/>
@@ -5990,45 +5990,45 @@
     </row>
     <row r="79" spans="2:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" s="17"/>
-      <c r="C79" s="33" t="s">
+      <c r="C79" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D79" s="33"/>
-      <c r="E79" s="33"/>
-      <c r="F79" s="33"/>
-      <c r="G79" s="33"/>
-      <c r="H79" s="33"/>
-      <c r="I79" s="33"/>
+      <c r="D79" s="32"/>
+      <c r="E79" s="32"/>
+      <c r="F79" s="32"/>
+      <c r="G79" s="32"/>
+      <c r="H79" s="32"/>
+      <c r="I79" s="32"/>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B80" s="17"/>
-      <c r="C80" s="33"/>
-      <c r="D80" s="33"/>
-      <c r="E80" s="33"/>
-      <c r="F80" s="33"/>
-      <c r="G80" s="33"/>
-      <c r="H80" s="33"/>
-      <c r="I80" s="33"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="32"/>
+      <c r="E80" s="32"/>
+      <c r="F80" s="32"/>
+      <c r="G80" s="32"/>
+      <c r="H80" s="32"/>
+      <c r="I80" s="32"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B81" s="17"/>
-      <c r="C81" s="33"/>
-      <c r="D81" s="33"/>
-      <c r="E81" s="33"/>
-      <c r="F81" s="33"/>
-      <c r="G81" s="33"/>
-      <c r="H81" s="33"/>
-      <c r="I81" s="33"/>
+      <c r="C81" s="32"/>
+      <c r="D81" s="32"/>
+      <c r="E81" s="32"/>
+      <c r="F81" s="32"/>
+      <c r="G81" s="32"/>
+      <c r="H81" s="32"/>
+      <c r="I81" s="32"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B82" s="17"/>
-      <c r="C82" s="33"/>
-      <c r="D82" s="33"/>
-      <c r="E82" s="33"/>
-      <c r="F82" s="33"/>
-      <c r="G82" s="33"/>
-      <c r="H82" s="33"/>
-      <c r="I82" s="33"/>
+      <c r="C82" s="32"/>
+      <c r="D82" s="32"/>
+      <c r="E82" s="32"/>
+      <c r="F82" s="32"/>
+      <c r="G82" s="32"/>
+      <c r="H82" s="32"/>
+      <c r="I82" s="32"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B83" s="17"/>
@@ -6053,46 +6053,46 @@
       <c r="B85" s="23"/>
     </row>
     <row r="86" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="33" t="s">
+      <c r="B86" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C86" s="33"/>
-      <c r="D86" s="33"/>
-      <c r="E86" s="33"/>
-      <c r="F86" s="33"/>
-      <c r="G86" s="33"/>
-      <c r="H86" s="33"/>
-      <c r="I86" s="33"/>
+      <c r="C86" s="32"/>
+      <c r="D86" s="32"/>
+      <c r="E86" s="32"/>
+      <c r="F86" s="32"/>
+      <c r="G86" s="32"/>
+      <c r="H86" s="32"/>
+      <c r="I86" s="32"/>
     </row>
     <row r="87" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B87" s="33"/>
-      <c r="C87" s="33"/>
-      <c r="D87" s="33"/>
-      <c r="E87" s="33"/>
-      <c r="F87" s="33"/>
-      <c r="G87" s="33"/>
-      <c r="H87" s="33"/>
-      <c r="I87" s="33"/>
+      <c r="B87" s="32"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="32"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="32"/>
+      <c r="G87" s="32"/>
+      <c r="H87" s="32"/>
+      <c r="I87" s="32"/>
     </row>
     <row r="88" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B88" s="33"/>
-      <c r="C88" s="33"/>
-      <c r="D88" s="33"/>
-      <c r="E88" s="33"/>
-      <c r="F88" s="33"/>
-      <c r="G88" s="33"/>
-      <c r="H88" s="33"/>
-      <c r="I88" s="33"/>
+      <c r="B88" s="32"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="32"/>
+      <c r="E88" s="32"/>
+      <c r="F88" s="32"/>
+      <c r="G88" s="32"/>
+      <c r="H88" s="32"/>
+      <c r="I88" s="32"/>
     </row>
     <row r="89" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="33"/>
-      <c r="C89" s="33"/>
-      <c r="D89" s="33"/>
-      <c r="E89" s="33"/>
-      <c r="F89" s="33"/>
-      <c r="G89" s="33"/>
-      <c r="H89" s="33"/>
-      <c r="I89" s="33"/>
+      <c r="B89" s="32"/>
+      <c r="C89" s="32"/>
+      <c r="D89" s="32"/>
+      <c r="E89" s="32"/>
+      <c r="F89" s="32"/>
+      <c r="G89" s="32"/>
+      <c r="H89" s="32"/>
+      <c r="I89" s="32"/>
     </row>
     <row r="90" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B90" s="13"/>
@@ -6105,26 +6105,26 @@
       <c r="I90" s="13"/>
     </row>
     <row r="91" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B91" s="33" t="s">
+      <c r="B91" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C91" s="33"/>
-      <c r="D91" s="33"/>
-      <c r="E91" s="33"/>
-      <c r="F91" s="33"/>
-      <c r="G91" s="33"/>
-      <c r="H91" s="33"/>
-      <c r="I91" s="33"/>
+      <c r="C91" s="32"/>
+      <c r="D91" s="32"/>
+      <c r="E91" s="32"/>
+      <c r="F91" s="32"/>
+      <c r="G91" s="32"/>
+      <c r="H91" s="32"/>
+      <c r="I91" s="32"/>
     </row>
     <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="33"/>
-      <c r="C92" s="33"/>
-      <c r="D92" s="33"/>
-      <c r="E92" s="33"/>
-      <c r="F92" s="33"/>
-      <c r="G92" s="33"/>
-      <c r="H92" s="33"/>
-      <c r="I92" s="33"/>
+      <c r="B92" s="32"/>
+      <c r="C92" s="32"/>
+      <c r="D92" s="32"/>
+      <c r="E92" s="32"/>
+      <c r="F92" s="32"/>
+      <c r="G92" s="32"/>
+      <c r="H92" s="32"/>
+      <c r="I92" s="32"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B93" s="20"/>
@@ -6137,113 +6137,113 @@
       <c r="I93" s="20"/>
     </row>
     <row r="94" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B94" s="33" t="s">
+      <c r="B94" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="C94" s="33"/>
-      <c r="D94" s="33"/>
-      <c r="E94" s="33"/>
-      <c r="F94" s="33"/>
-      <c r="G94" s="33"/>
-      <c r="H94" s="33"/>
-      <c r="I94" s="33"/>
+      <c r="C94" s="32"/>
+      <c r="D94" s="32"/>
+      <c r="E94" s="32"/>
+      <c r="F94" s="32"/>
+      <c r="G94" s="32"/>
+      <c r="H94" s="32"/>
+      <c r="I94" s="32"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B95" s="33"/>
-      <c r="C95" s="33"/>
-      <c r="D95" s="33"/>
-      <c r="E95" s="33"/>
-      <c r="F95" s="33"/>
-      <c r="G95" s="33"/>
-      <c r="H95" s="33"/>
-      <c r="I95" s="33"/>
+      <c r="B95" s="32"/>
+      <c r="C95" s="32"/>
+      <c r="D95" s="32"/>
+      <c r="E95" s="32"/>
+      <c r="F95" s="32"/>
+      <c r="G95" s="32"/>
+      <c r="H95" s="32"/>
+      <c r="I95" s="32"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B96" s="33"/>
-      <c r="C96" s="33"/>
-      <c r="D96" s="33"/>
-      <c r="E96" s="33"/>
-      <c r="F96" s="33"/>
-      <c r="G96" s="33"/>
-      <c r="H96" s="33"/>
-      <c r="I96" s="33"/>
+      <c r="B96" s="32"/>
+      <c r="C96" s="32"/>
+      <c r="D96" s="32"/>
+      <c r="E96" s="32"/>
+      <c r="F96" s="32"/>
+      <c r="G96" s="32"/>
+      <c r="H96" s="32"/>
+      <c r="I96" s="32"/>
     </row>
     <row r="98" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="6">
         <v>6</v>
       </c>
-      <c r="B98" s="35" t="s">
+      <c r="B98" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C98" s="35"/>
-      <c r="D98" s="35"/>
-      <c r="E98" s="35"/>
-      <c r="F98" s="35"/>
-      <c r="G98" s="35"/>
-      <c r="H98" s="35"/>
-      <c r="I98" s="35"/>
+      <c r="C98" s="34"/>
+      <c r="D98" s="34"/>
+      <c r="E98" s="34"/>
+      <c r="F98" s="34"/>
+      <c r="G98" s="34"/>
+      <c r="H98" s="34"/>
+      <c r="I98" s="34"/>
     </row>
     <row r="99" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B99" s="33" t="s">
+      <c r="B99" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C99" s="33"/>
-      <c r="D99" s="33"/>
-      <c r="E99" s="33"/>
-      <c r="F99" s="33"/>
-      <c r="G99" s="33"/>
-      <c r="H99" s="33"/>
-      <c r="I99" s="33"/>
+      <c r="C99" s="32"/>
+      <c r="D99" s="32"/>
+      <c r="E99" s="32"/>
+      <c r="F99" s="32"/>
+      <c r="G99" s="32"/>
+      <c r="H99" s="32"/>
+      <c r="I99" s="32"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B100" s="33"/>
-      <c r="C100" s="33"/>
-      <c r="D100" s="33"/>
-      <c r="E100" s="33"/>
-      <c r="F100" s="33"/>
-      <c r="G100" s="33"/>
-      <c r="H100" s="33"/>
-      <c r="I100" s="33"/>
+      <c r="B100" s="32"/>
+      <c r="C100" s="32"/>
+      <c r="D100" s="32"/>
+      <c r="E100" s="32"/>
+      <c r="F100" s="32"/>
+      <c r="G100" s="32"/>
+      <c r="H100" s="32"/>
+      <c r="I100" s="32"/>
     </row>
     <row r="101" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B101" s="33"/>
-      <c r="C101" s="33"/>
-      <c r="D101" s="33"/>
-      <c r="E101" s="33"/>
-      <c r="F101" s="33"/>
-      <c r="G101" s="33"/>
-      <c r="H101" s="33"/>
-      <c r="I101" s="33"/>
+      <c r="B101" s="32"/>
+      <c r="C101" s="32"/>
+      <c r="D101" s="32"/>
+      <c r="E101" s="32"/>
+      <c r="F101" s="32"/>
+      <c r="G101" s="32"/>
+      <c r="H101" s="32"/>
+      <c r="I101" s="32"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B102" s="33"/>
-      <c r="C102" s="33"/>
-      <c r="D102" s="33"/>
-      <c r="E102" s="33"/>
-      <c r="F102" s="33"/>
-      <c r="G102" s="33"/>
-      <c r="H102" s="33"/>
-      <c r="I102" s="33"/>
+      <c r="B102" s="32"/>
+      <c r="C102" s="32"/>
+      <c r="D102" s="32"/>
+      <c r="E102" s="32"/>
+      <c r="F102" s="32"/>
+      <c r="G102" s="32"/>
+      <c r="H102" s="32"/>
+      <c r="I102" s="32"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B103" s="33"/>
-      <c r="C103" s="33"/>
-      <c r="D103" s="33"/>
-      <c r="E103" s="33"/>
-      <c r="F103" s="33"/>
-      <c r="G103" s="33"/>
-      <c r="H103" s="33"/>
-      <c r="I103" s="33"/>
+      <c r="B103" s="32"/>
+      <c r="C103" s="32"/>
+      <c r="D103" s="32"/>
+      <c r="E103" s="32"/>
+      <c r="F103" s="32"/>
+      <c r="G103" s="32"/>
+      <c r="H103" s="32"/>
+      <c r="I103" s="32"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B104" s="33"/>
-      <c r="C104" s="33"/>
-      <c r="D104" s="33"/>
-      <c r="E104" s="33"/>
-      <c r="F104" s="33"/>
-      <c r="G104" s="33"/>
-      <c r="H104" s="33"/>
-      <c r="I104" s="33"/>
+      <c r="B104" s="32"/>
+      <c r="C104" s="32"/>
+      <c r="D104" s="32"/>
+      <c r="E104" s="32"/>
+      <c r="F104" s="32"/>
+      <c r="G104" s="32"/>
+      <c r="H104" s="32"/>
+      <c r="I104" s="32"/>
     </row>
     <row r="105" spans="1:9" ht="20" x14ac:dyDescent="0.4">
       <c r="B105" s="2" t="s">
@@ -6271,76 +6271,76 @@
       <c r="B114"/>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="G115" s="34" t="s">
+      <c r="G115" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="H115" s="34"/>
-      <c r="I115" s="34"/>
+      <c r="H115" s="31"/>
+      <c r="I115" s="31"/>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="G116" s="34"/>
-      <c r="H116" s="34"/>
-      <c r="I116" s="34"/>
+      <c r="G116" s="31"/>
+      <c r="H116" s="31"/>
+      <c r="I116" s="31"/>
     </row>
     <row r="117" spans="2:9" ht="20" x14ac:dyDescent="0.4">
       <c r="G117"/>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="H118" s="34" t="s">
+      <c r="H118" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="I118" s="34"/>
+      <c r="I118" s="31"/>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="H119" s="34"/>
-      <c r="I119" s="34"/>
+      <c r="H119" s="31"/>
+      <c r="I119" s="31"/>
     </row>
     <row r="120" spans="2:9" ht="20" x14ac:dyDescent="0.4">
       <c r="G120"/>
     </row>
     <row r="121" spans="2:9" ht="20" x14ac:dyDescent="0.4">
       <c r="G121"/>
-      <c r="H121" s="34" t="s">
+      <c r="H121" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="I121" s="34"/>
+      <c r="I121" s="31"/>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="H122" s="34"/>
-      <c r="I122" s="34"/>
+      <c r="H122" s="31"/>
+      <c r="I122" s="31"/>
     </row>
     <row r="135" spans="1:9" ht="20" x14ac:dyDescent="0.4">
       <c r="A135"/>
-      <c r="B135" s="33" t="s">
+      <c r="B135" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C135" s="33"/>
-      <c r="D135" s="33"/>
-      <c r="E135" s="33"/>
-      <c r="F135" s="33"/>
-      <c r="G135" s="33"/>
-      <c r="H135" s="33"/>
-      <c r="I135" s="33"/>
+      <c r="C135" s="32"/>
+      <c r="D135" s="32"/>
+      <c r="E135" s="32"/>
+      <c r="F135" s="32"/>
+      <c r="G135" s="32"/>
+      <c r="H135" s="32"/>
+      <c r="I135" s="32"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B136" s="33"/>
-      <c r="C136" s="33"/>
-      <c r="D136" s="33"/>
-      <c r="E136" s="33"/>
-      <c r="F136" s="33"/>
-      <c r="G136" s="33"/>
-      <c r="H136" s="33"/>
-      <c r="I136" s="33"/>
+      <c r="B136" s="32"/>
+      <c r="C136" s="32"/>
+      <c r="D136" s="32"/>
+      <c r="E136" s="32"/>
+      <c r="F136" s="32"/>
+      <c r="G136" s="32"/>
+      <c r="H136" s="32"/>
+      <c r="I136" s="32"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B137" s="33"/>
-      <c r="C137" s="33"/>
-      <c r="D137" s="33"/>
-      <c r="E137" s="33"/>
-      <c r="F137" s="33"/>
-      <c r="G137" s="33"/>
-      <c r="H137" s="33"/>
-      <c r="I137" s="33"/>
+      <c r="B137" s="32"/>
+      <c r="C137" s="32"/>
+      <c r="D137" s="32"/>
+      <c r="E137" s="32"/>
+      <c r="F137" s="32"/>
+      <c r="G137" s="32"/>
+      <c r="H137" s="32"/>
+      <c r="I137" s="32"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B139" s="2" t="s">
@@ -6348,26 +6348,26 @@
       </c>
     </row>
     <row r="140" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B140" s="34" t="s">
+      <c r="B140" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C140" s="34"/>
-      <c r="D140" s="34"/>
-      <c r="E140" s="34"/>
-      <c r="F140" s="34"/>
-      <c r="G140" s="34"/>
-      <c r="H140" s="34"/>
-      <c r="I140" s="34"/>
+      <c r="C140" s="31"/>
+      <c r="D140" s="31"/>
+      <c r="E140" s="31"/>
+      <c r="F140" s="31"/>
+      <c r="G140" s="31"/>
+      <c r="H140" s="31"/>
+      <c r="I140" s="31"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B141" s="34"/>
-      <c r="C141" s="34"/>
-      <c r="D141" s="34"/>
-      <c r="E141" s="34"/>
-      <c r="F141" s="34"/>
-      <c r="G141" s="34"/>
-      <c r="H141" s="34"/>
-      <c r="I141" s="34"/>
+      <c r="B141" s="31"/>
+      <c r="C141" s="31"/>
+      <c r="D141" s="31"/>
+      <c r="E141" s="31"/>
+      <c r="F141" s="31"/>
+      <c r="G141" s="31"/>
+      <c r="H141" s="31"/>
+      <c r="I141" s="31"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B142" s="25"/>
@@ -6383,47 +6383,47 @@
       <c r="A143" s="6">
         <v>7</v>
       </c>
-      <c r="B143" s="34" t="s">
+      <c r="B143" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C143" s="34"/>
-      <c r="D143" s="34"/>
-      <c r="E143" s="34"/>
-      <c r="F143" s="34"/>
-      <c r="G143" s="34"/>
-      <c r="H143" s="34"/>
-      <c r="I143" s="34"/>
+      <c r="C143" s="31"/>
+      <c r="D143" s="31"/>
+      <c r="E143" s="31"/>
+      <c r="F143" s="31"/>
+      <c r="G143" s="31"/>
+      <c r="H143" s="31"/>
+      <c r="I143" s="31"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B144" s="34"/>
-      <c r="C144" s="34"/>
-      <c r="D144" s="34"/>
-      <c r="E144" s="34"/>
-      <c r="F144" s="34"/>
-      <c r="G144" s="34"/>
-      <c r="H144" s="34"/>
-      <c r="I144" s="34"/>
+      <c r="B144" s="31"/>
+      <c r="C144" s="31"/>
+      <c r="D144" s="31"/>
+      <c r="E144" s="31"/>
+      <c r="F144" s="31"/>
+      <c r="G144" s="31"/>
+      <c r="H144" s="31"/>
+      <c r="I144" s="31"/>
     </row>
     <row r="145" spans="1:9" ht="20" x14ac:dyDescent="0.4">
       <c r="B145"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H146" s="34" t="s">
+      <c r="H146" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="I146" s="34"/>
+      <c r="I146" s="31"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H147" s="34"/>
-      <c r="I147" s="34"/>
+      <c r="H147" s="31"/>
+      <c r="I147" s="31"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H148" s="34"/>
-      <c r="I148" s="34"/>
+      <c r="H148" s="31"/>
+      <c r="I148" s="31"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H149" s="34"/>
-      <c r="I149" s="34"/>
+      <c r="H149" s="31"/>
+      <c r="I149" s="31"/>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B151" s="2" t="s">
@@ -6432,62 +6432,62 @@
     </row>
     <row r="153" spans="1:9" ht="20" x14ac:dyDescent="0.4">
       <c r="A153"/>
-      <c r="B153" s="34" t="s">
+      <c r="B153" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C153" s="34"/>
-      <c r="D153" s="34"/>
-      <c r="E153" s="34"/>
-      <c r="F153" s="34"/>
-      <c r="G153" s="34"/>
-      <c r="H153" s="34"/>
-      <c r="I153" s="34"/>
+      <c r="C153" s="31"/>
+      <c r="D153" s="31"/>
+      <c r="E153" s="31"/>
+      <c r="F153" s="31"/>
+      <c r="G153" s="31"/>
+      <c r="H153" s="31"/>
+      <c r="I153" s="31"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B154" s="34"/>
-      <c r="C154" s="34"/>
-      <c r="D154" s="34"/>
-      <c r="E154" s="34"/>
-      <c r="F154" s="34"/>
-      <c r="G154" s="34"/>
-      <c r="H154" s="34"/>
-      <c r="I154" s="34"/>
+      <c r="B154" s="31"/>
+      <c r="C154" s="31"/>
+      <c r="D154" s="31"/>
+      <c r="E154" s="31"/>
+      <c r="F154" s="31"/>
+      <c r="G154" s="31"/>
+      <c r="H154" s="31"/>
+      <c r="I154" s="31"/>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B155" s="34"/>
-      <c r="C155" s="34"/>
-      <c r="D155" s="34"/>
-      <c r="E155" s="34"/>
-      <c r="F155" s="34"/>
-      <c r="G155" s="34"/>
-      <c r="H155" s="34"/>
-      <c r="I155" s="34"/>
+      <c r="B155" s="31"/>
+      <c r="C155" s="31"/>
+      <c r="D155" s="31"/>
+      <c r="E155" s="31"/>
+      <c r="F155" s="31"/>
+      <c r="G155" s="31"/>
+      <c r="H155" s="31"/>
+      <c r="I155" s="31"/>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F157" s="34" t="s">
+      <c r="F157" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="G157" s="34"/>
-      <c r="H157" s="34"/>
-      <c r="I157" s="34"/>
+      <c r="G157" s="31"/>
+      <c r="H157" s="31"/>
+      <c r="I157" s="31"/>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F158" s="34"/>
-      <c r="G158" s="34"/>
-      <c r="H158" s="34"/>
-      <c r="I158" s="34"/>
+      <c r="F158" s="31"/>
+      <c r="G158" s="31"/>
+      <c r="H158" s="31"/>
+      <c r="I158" s="31"/>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F159" s="34"/>
-      <c r="G159" s="34"/>
-      <c r="H159" s="34"/>
-      <c r="I159" s="34"/>
+      <c r="F159" s="31"/>
+      <c r="G159" s="31"/>
+      <c r="H159" s="31"/>
+      <c r="I159" s="31"/>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="F160" s="34"/>
-      <c r="G160" s="34"/>
-      <c r="H160" s="34"/>
-      <c r="I160" s="34"/>
+      <c r="F160" s="31"/>
+      <c r="G160" s="31"/>
+      <c r="H160" s="31"/>
+      <c r="I160" s="31"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B165" s="19"/>
@@ -6503,16 +6503,16 @@
       <c r="A166" s="6">
         <v>8</v>
       </c>
-      <c r="B166" s="35" t="s">
+      <c r="B166" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C166" s="35"/>
-      <c r="D166" s="35"/>
-      <c r="E166" s="35"/>
-      <c r="F166" s="35"/>
-      <c r="G166" s="35"/>
-      <c r="H166" s="35"/>
-      <c r="I166" s="35"/>
+      <c r="C166" s="34"/>
+      <c r="D166" s="34"/>
+      <c r="E166" s="34"/>
+      <c r="F166" s="34"/>
+      <c r="G166" s="34"/>
+      <c r="H166" s="34"/>
+      <c r="I166" s="34"/>
     </row>
     <row r="167" spans="1:9" ht="20" x14ac:dyDescent="0.4">
       <c r="F167"/>
@@ -6529,26 +6529,26 @@
       <c r="B169"/>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B175" s="34" t="s">
+      <c r="B175" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C175" s="34"/>
-      <c r="D175" s="34"/>
-      <c r="E175" s="34"/>
-      <c r="F175" s="34"/>
-      <c r="G175" s="34"/>
-      <c r="H175" s="34"/>
-      <c r="I175" s="34"/>
+      <c r="C175" s="31"/>
+      <c r="D175" s="31"/>
+      <c r="E175" s="31"/>
+      <c r="F175" s="31"/>
+      <c r="G175" s="31"/>
+      <c r="H175" s="31"/>
+      <c r="I175" s="31"/>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B176" s="34"/>
-      <c r="C176" s="34"/>
-      <c r="D176" s="34"/>
-      <c r="E176" s="34"/>
-      <c r="F176" s="34"/>
-      <c r="G176" s="34"/>
-      <c r="H176" s="34"/>
-      <c r="I176" s="34"/>
+      <c r="B176" s="31"/>
+      <c r="C176" s="31"/>
+      <c r="D176" s="31"/>
+      <c r="E176" s="31"/>
+      <c r="F176" s="31"/>
+      <c r="G176" s="31"/>
+      <c r="H176" s="31"/>
+      <c r="I176" s="31"/>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B177" s="21"/>
@@ -6564,26 +6564,26 @@
       <c r="A179" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B179" s="34" t="s">
+      <c r="B179" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="C179" s="34"/>
-      <c r="D179" s="34"/>
-      <c r="E179" s="34"/>
-      <c r="F179" s="34"/>
-      <c r="G179" s="34"/>
-      <c r="H179" s="34"/>
-      <c r="I179" s="34"/>
+      <c r="C179" s="31"/>
+      <c r="D179" s="31"/>
+      <c r="E179" s="31"/>
+      <c r="F179" s="31"/>
+      <c r="G179" s="31"/>
+      <c r="H179" s="31"/>
+      <c r="I179" s="31"/>
     </row>
     <row r="180" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B180" s="34"/>
-      <c r="C180" s="34"/>
-      <c r="D180" s="34"/>
-      <c r="E180" s="34"/>
-      <c r="F180" s="34"/>
-      <c r="G180" s="34"/>
-      <c r="H180" s="34"/>
-      <c r="I180" s="34"/>
+      <c r="B180" s="31"/>
+      <c r="C180" s="31"/>
+      <c r="D180" s="31"/>
+      <c r="E180" s="31"/>
+      <c r="F180" s="31"/>
+      <c r="G180" s="31"/>
+      <c r="H180" s="31"/>
+      <c r="I180" s="31"/>
     </row>
     <row r="181" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A181"/>
@@ -6593,119 +6593,119 @@
       <c r="A192" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B192" s="34" t="s">
+      <c r="B192" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C192" s="34"/>
-      <c r="D192" s="34"/>
-      <c r="E192" s="34"/>
-      <c r="F192" s="34"/>
-      <c r="G192" s="34"/>
-      <c r="H192" s="34"/>
-      <c r="I192" s="34"/>
+      <c r="C192" s="31"/>
+      <c r="D192" s="31"/>
+      <c r="E192" s="31"/>
+      <c r="F192" s="31"/>
+      <c r="G192" s="31"/>
+      <c r="H192" s="31"/>
+      <c r="I192" s="31"/>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B193" s="34"/>
-      <c r="C193" s="34"/>
-      <c r="D193" s="34"/>
-      <c r="E193" s="34"/>
-      <c r="F193" s="34"/>
-      <c r="G193" s="34"/>
-      <c r="H193" s="34"/>
-      <c r="I193" s="34"/>
+      <c r="B193" s="31"/>
+      <c r="C193" s="31"/>
+      <c r="D193" s="31"/>
+      <c r="E193" s="31"/>
+      <c r="F193" s="31"/>
+      <c r="G193" s="31"/>
+      <c r="H193" s="31"/>
+      <c r="I193" s="31"/>
     </row>
     <row r="197" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="202" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A202" s="6">
         <v>9</v>
       </c>
-      <c r="B202" s="35" t="s">
+      <c r="B202" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C202" s="35"/>
-      <c r="D202" s="35"/>
-      <c r="E202" s="35"/>
-      <c r="F202" s="35"/>
-      <c r="G202" s="35"/>
-      <c r="H202" s="35"/>
-      <c r="I202" s="35"/>
+      <c r="C202" s="34"/>
+      <c r="D202" s="34"/>
+      <c r="E202" s="34"/>
+      <c r="F202" s="34"/>
+      <c r="G202" s="34"/>
+      <c r="H202" s="34"/>
+      <c r="I202" s="34"/>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B203" s="34" t="s">
+      <c r="B203" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C203" s="34"/>
-      <c r="D203" s="34"/>
-      <c r="E203" s="34"/>
-      <c r="F203" s="34"/>
-      <c r="G203" s="34"/>
-      <c r="H203" s="34"/>
-      <c r="I203" s="34"/>
+      <c r="C203" s="31"/>
+      <c r="D203" s="31"/>
+      <c r="E203" s="31"/>
+      <c r="F203" s="31"/>
+      <c r="G203" s="31"/>
+      <c r="H203" s="31"/>
+      <c r="I203" s="31"/>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B204" s="34"/>
-      <c r="C204" s="34"/>
-      <c r="D204" s="34"/>
-      <c r="E204" s="34"/>
-      <c r="F204" s="34"/>
-      <c r="G204" s="34"/>
-      <c r="H204" s="34"/>
-      <c r="I204" s="34"/>
+      <c r="B204" s="31"/>
+      <c r="C204" s="31"/>
+      <c r="D204" s="31"/>
+      <c r="E204" s="31"/>
+      <c r="F204" s="31"/>
+      <c r="G204" s="31"/>
+      <c r="H204" s="31"/>
+      <c r="I204" s="31"/>
     </row>
     <row r="205" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B205"/>
     </row>
     <row r="206" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B206" s="31" t="s">
+      <c r="B206" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="C206" s="31"/>
-      <c r="D206" s="31"/>
-      <c r="E206" s="31"/>
-      <c r="F206" s="31"/>
-      <c r="G206" s="31"/>
-      <c r="H206" s="31"/>
-      <c r="I206" s="31"/>
+      <c r="C206" s="44"/>
+      <c r="D206" s="44"/>
+      <c r="E206" s="44"/>
+      <c r="F206" s="44"/>
+      <c r="G206" s="44"/>
+      <c r="H206" s="44"/>
+      <c r="I206" s="44"/>
     </row>
     <row r="207" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B207" s="31"/>
-      <c r="C207" s="31"/>
-      <c r="D207" s="31"/>
-      <c r="E207" s="31"/>
-      <c r="F207" s="31"/>
-      <c r="G207" s="31"/>
-      <c r="H207" s="31"/>
-      <c r="I207" s="31"/>
+      <c r="B207" s="44"/>
+      <c r="C207" s="44"/>
+      <c r="D207" s="44"/>
+      <c r="E207" s="44"/>
+      <c r="F207" s="44"/>
+      <c r="G207" s="44"/>
+      <c r="H207" s="44"/>
+      <c r="I207" s="44"/>
     </row>
     <row r="208" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B208" s="31"/>
-      <c r="C208" s="31"/>
-      <c r="D208" s="31"/>
-      <c r="E208" s="31"/>
-      <c r="F208" s="31"/>
-      <c r="G208" s="31"/>
-      <c r="H208" s="31"/>
-      <c r="I208" s="31"/>
+      <c r="B208" s="44"/>
+      <c r="C208" s="44"/>
+      <c r="D208" s="44"/>
+      <c r="E208" s="44"/>
+      <c r="F208" s="44"/>
+      <c r="G208" s="44"/>
+      <c r="H208" s="44"/>
+      <c r="I208" s="44"/>
     </row>
     <row r="209" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B209" s="31"/>
-      <c r="C209" s="31"/>
-      <c r="D209" s="31"/>
-      <c r="E209" s="31"/>
-      <c r="F209" s="31"/>
-      <c r="G209" s="31"/>
-      <c r="H209" s="31"/>
-      <c r="I209" s="31"/>
+      <c r="B209" s="44"/>
+      <c r="C209" s="44"/>
+      <c r="D209" s="44"/>
+      <c r="E209" s="44"/>
+      <c r="F209" s="44"/>
+      <c r="G209" s="44"/>
+      <c r="H209" s="44"/>
+      <c r="I209" s="44"/>
     </row>
     <row r="210" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B210" s="31"/>
-      <c r="C210" s="31"/>
-      <c r="D210" s="31"/>
-      <c r="E210" s="31"/>
-      <c r="F210" s="31"/>
-      <c r="G210" s="31"/>
-      <c r="H210" s="31"/>
-      <c r="I210" s="31"/>
+      <c r="B210" s="44"/>
+      <c r="C210" s="44"/>
+      <c r="D210" s="44"/>
+      <c r="E210" s="44"/>
+      <c r="F210" s="44"/>
+      <c r="G210" s="44"/>
+      <c r="H210" s="44"/>
+      <c r="I210" s="44"/>
     </row>
     <row r="211" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B211"/>
@@ -6717,148 +6717,148 @@
       <c r="A213" s="6">
         <v>10</v>
       </c>
-      <c r="B213" s="35" t="s">
+      <c r="B213" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C213" s="35"/>
-      <c r="D213" s="35"/>
-      <c r="E213" s="35"/>
-      <c r="F213" s="35"/>
-      <c r="G213" s="35"/>
-      <c r="H213" s="35"/>
-      <c r="I213" s="35"/>
+      <c r="C213" s="34"/>
+      <c r="D213" s="34"/>
+      <c r="E213" s="34"/>
+      <c r="F213" s="34"/>
+      <c r="G213" s="34"/>
+      <c r="H213" s="34"/>
+      <c r="I213" s="34"/>
     </row>
     <row r="214" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B214" s="34" t="s">
+      <c r="B214" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C214" s="34"/>
+      <c r="C214" s="31"/>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B215" s="34"/>
-      <c r="C215" s="34"/>
+      <c r="B215" s="31"/>
+      <c r="C215" s="31"/>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B216" s="34"/>
-      <c r="C216" s="34"/>
+      <c r="B216" s="31"/>
+      <c r="C216" s="31"/>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B217" s="34"/>
-      <c r="C217" s="34"/>
+      <c r="B217" s="31"/>
+      <c r="C217" s="31"/>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B218" s="34"/>
-      <c r="C218" s="34"/>
+      <c r="B218" s="31"/>
+      <c r="C218" s="31"/>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B219" s="34"/>
-      <c r="C219" s="34"/>
+      <c r="B219" s="31"/>
+      <c r="C219" s="31"/>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B220" s="34"/>
-      <c r="C220" s="34"/>
+      <c r="B220" s="31"/>
+      <c r="C220" s="31"/>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A228" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="B228" s="33" t="s">
+      <c r="B228" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="C228" s="33"/>
-      <c r="D228" s="33"/>
-      <c r="E228" s="33"/>
-      <c r="F228" s="33"/>
-      <c r="G228" s="33"/>
-      <c r="H228" s="33"/>
-      <c r="I228" s="33"/>
+      <c r="C228" s="32"/>
+      <c r="D228" s="32"/>
+      <c r="E228" s="32"/>
+      <c r="F228" s="32"/>
+      <c r="G228" s="32"/>
+      <c r="H228" s="32"/>
+      <c r="I228" s="32"/>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B229" s="33"/>
-      <c r="C229" s="33"/>
-      <c r="D229" s="33"/>
-      <c r="E229" s="33"/>
-      <c r="F229" s="33"/>
-      <c r="G229" s="33"/>
-      <c r="H229" s="33"/>
-      <c r="I229" s="33"/>
+      <c r="B229" s="32"/>
+      <c r="C229" s="32"/>
+      <c r="D229" s="32"/>
+      <c r="E229" s="32"/>
+      <c r="F229" s="32"/>
+      <c r="G229" s="32"/>
+      <c r="H229" s="32"/>
+      <c r="I229" s="32"/>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B230" s="33"/>
-      <c r="C230" s="33"/>
-      <c r="D230" s="33"/>
-      <c r="E230" s="33"/>
-      <c r="F230" s="33"/>
-      <c r="G230" s="33"/>
-      <c r="H230" s="33"/>
-      <c r="I230" s="33"/>
+      <c r="B230" s="32"/>
+      <c r="C230" s="32"/>
+      <c r="D230" s="32"/>
+      <c r="E230" s="32"/>
+      <c r="F230" s="32"/>
+      <c r="G230" s="32"/>
+      <c r="H230" s="32"/>
+      <c r="I230" s="32"/>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B231" s="33"/>
-      <c r="C231" s="33"/>
-      <c r="D231" s="33"/>
-      <c r="E231" s="33"/>
-      <c r="F231" s="33"/>
-      <c r="G231" s="33"/>
-      <c r="H231" s="33"/>
-      <c r="I231" s="33"/>
+      <c r="B231" s="32"/>
+      <c r="C231" s="32"/>
+      <c r="D231" s="32"/>
+      <c r="E231" s="32"/>
+      <c r="F231" s="32"/>
+      <c r="G231" s="32"/>
+      <c r="H231" s="32"/>
+      <c r="I231" s="32"/>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B232" s="33"/>
-      <c r="C232" s="33"/>
-      <c r="D232" s="33"/>
-      <c r="E232" s="33"/>
-      <c r="F232" s="33"/>
-      <c r="G232" s="33"/>
-      <c r="H232" s="33"/>
-      <c r="I232" s="33"/>
+      <c r="B232" s="32"/>
+      <c r="C232" s="32"/>
+      <c r="D232" s="32"/>
+      <c r="E232" s="32"/>
+      <c r="F232" s="32"/>
+      <c r="G232" s="32"/>
+      <c r="H232" s="32"/>
+      <c r="I232" s="32"/>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A234" s="6">
         <v>11</v>
       </c>
-      <c r="B234" s="35" t="s">
+      <c r="B234" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C234" s="35"/>
-      <c r="D234" s="35"/>
-      <c r="E234" s="35"/>
-      <c r="F234" s="35"/>
-      <c r="G234" s="35"/>
-      <c r="H234" s="35"/>
-      <c r="I234" s="35"/>
+      <c r="C234" s="34"/>
+      <c r="D234" s="34"/>
+      <c r="E234" s="34"/>
+      <c r="F234" s="34"/>
+      <c r="G234" s="34"/>
+      <c r="H234" s="34"/>
+      <c r="I234" s="34"/>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B235" s="34" t="s">
+      <c r="B235" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C235" s="34"/>
-      <c r="D235" s="34"/>
-      <c r="E235" s="34"/>
-      <c r="F235" s="34"/>
-      <c r="G235" s="34"/>
-      <c r="H235" s="34"/>
-      <c r="I235" s="34"/>
+      <c r="C235" s="31"/>
+      <c r="D235" s="31"/>
+      <c r="E235" s="31"/>
+      <c r="F235" s="31"/>
+      <c r="G235" s="31"/>
+      <c r="H235" s="31"/>
+      <c r="I235" s="31"/>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B236" s="34"/>
-      <c r="C236" s="34"/>
-      <c r="D236" s="34"/>
-      <c r="E236" s="34"/>
-      <c r="F236" s="34"/>
-      <c r="G236" s="34"/>
-      <c r="H236" s="34"/>
-      <c r="I236" s="34"/>
+      <c r="B236" s="31"/>
+      <c r="C236" s="31"/>
+      <c r="D236" s="31"/>
+      <c r="E236" s="31"/>
+      <c r="F236" s="31"/>
+      <c r="G236" s="31"/>
+      <c r="H236" s="31"/>
+      <c r="I236" s="31"/>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B237" s="34"/>
-      <c r="C237" s="34"/>
-      <c r="D237" s="34"/>
-      <c r="E237" s="34"/>
-      <c r="F237" s="34"/>
-      <c r="G237" s="34"/>
-      <c r="H237" s="34"/>
-      <c r="I237" s="34"/>
+      <c r="B237" s="31"/>
+      <c r="C237" s="31"/>
+      <c r="D237" s="31"/>
+      <c r="E237" s="31"/>
+      <c r="F237" s="31"/>
+      <c r="G237" s="31"/>
+      <c r="H237" s="31"/>
+      <c r="I237" s="31"/>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B238" s="19"/>
@@ -6884,120 +6884,120 @@
       <c r="A240" s="6">
         <v>12</v>
       </c>
-      <c r="B240" s="35" t="s">
+      <c r="B240" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C240" s="35"/>
-      <c r="D240" s="35"/>
-      <c r="E240" s="35"/>
-      <c r="F240" s="35"/>
-      <c r="G240" s="35"/>
-      <c r="H240" s="35"/>
-      <c r="I240" s="35"/>
+      <c r="C240" s="34"/>
+      <c r="D240" s="34"/>
+      <c r="E240" s="34"/>
+      <c r="F240" s="34"/>
+      <c r="G240" s="34"/>
+      <c r="H240" s="34"/>
+      <c r="I240" s="34"/>
     </row>
     <row r="241" spans="1:9" ht="20" x14ac:dyDescent="0.4">
       <c r="A241"/>
-      <c r="B241" s="33" t="s">
+      <c r="B241" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C241" s="33"/>
-      <c r="D241" s="33"/>
-      <c r="E241" s="33"/>
-      <c r="F241" s="33"/>
-      <c r="G241" s="33"/>
-      <c r="H241" s="33"/>
-      <c r="I241" s="33"/>
+      <c r="C241" s="32"/>
+      <c r="D241" s="32"/>
+      <c r="E241" s="32"/>
+      <c r="F241" s="32"/>
+      <c r="G241" s="32"/>
+      <c r="H241" s="32"/>
+      <c r="I241" s="32"/>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B242" s="33"/>
-      <c r="C242" s="33"/>
-      <c r="D242" s="33"/>
-      <c r="E242" s="33"/>
-      <c r="F242" s="33"/>
-      <c r="G242" s="33"/>
-      <c r="H242" s="33"/>
-      <c r="I242" s="33"/>
+      <c r="B242" s="32"/>
+      <c r="C242" s="32"/>
+      <c r="D242" s="32"/>
+      <c r="E242" s="32"/>
+      <c r="F242" s="32"/>
+      <c r="G242" s="32"/>
+      <c r="H242" s="32"/>
+      <c r="I242" s="32"/>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B243" s="33"/>
-      <c r="C243" s="33"/>
-      <c r="D243" s="33"/>
-      <c r="E243" s="33"/>
-      <c r="F243" s="33"/>
-      <c r="G243" s="33"/>
-      <c r="H243" s="33"/>
-      <c r="I243" s="33"/>
+      <c r="B243" s="32"/>
+      <c r="C243" s="32"/>
+      <c r="D243" s="32"/>
+      <c r="E243" s="32"/>
+      <c r="F243" s="32"/>
+      <c r="G243" s="32"/>
+      <c r="H243" s="32"/>
+      <c r="I243" s="32"/>
     </row>
     <row r="244" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B244" s="33"/>
-      <c r="C244" s="33"/>
-      <c r="D244" s="33"/>
-      <c r="E244" s="33"/>
-      <c r="F244" s="33"/>
-      <c r="G244" s="33"/>
-      <c r="H244" s="33"/>
-      <c r="I244" s="33"/>
+      <c r="B244" s="32"/>
+      <c r="C244" s="32"/>
+      <c r="D244" s="32"/>
+      <c r="E244" s="32"/>
+      <c r="F244" s="32"/>
+      <c r="G244" s="32"/>
+      <c r="H244" s="32"/>
+      <c r="I244" s="32"/>
     </row>
     <row r="246" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="266" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A266" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B266" s="34" t="s">
+      <c r="B266" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C266" s="34"/>
-      <c r="D266" s="34"/>
-      <c r="E266" s="34"/>
-      <c r="F266" s="34"/>
-      <c r="G266" s="34"/>
-      <c r="H266" s="34"/>
-      <c r="I266" s="34"/>
+      <c r="C266" s="31"/>
+      <c r="D266" s="31"/>
+      <c r="E266" s="31"/>
+      <c r="F266" s="31"/>
+      <c r="G266" s="31"/>
+      <c r="H266" s="31"/>
+      <c r="I266" s="31"/>
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B267" s="34"/>
-      <c r="C267" s="34"/>
-      <c r="D267" s="34"/>
-      <c r="E267" s="34"/>
-      <c r="F267" s="34"/>
-      <c r="G267" s="34"/>
-      <c r="H267" s="34"/>
-      <c r="I267" s="34"/>
+      <c r="B267" s="31"/>
+      <c r="C267" s="31"/>
+      <c r="D267" s="31"/>
+      <c r="E267" s="31"/>
+      <c r="F267" s="31"/>
+      <c r="G267" s="31"/>
+      <c r="H267" s="31"/>
+      <c r="I267" s="31"/>
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B268" s="34"/>
-      <c r="C268" s="34"/>
-      <c r="D268" s="34"/>
-      <c r="E268" s="34"/>
-      <c r="F268" s="34"/>
-      <c r="G268" s="34"/>
-      <c r="H268" s="34"/>
-      <c r="I268" s="34"/>
+      <c r="B268" s="31"/>
+      <c r="C268" s="31"/>
+      <c r="D268" s="31"/>
+      <c r="E268" s="31"/>
+      <c r="F268" s="31"/>
+      <c r="G268" s="31"/>
+      <c r="H268" s="31"/>
+      <c r="I268" s="31"/>
     </row>
     <row r="270" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A270" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B270" s="34" t="s">
+      <c r="B270" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C270" s="34"/>
-      <c r="D270" s="34"/>
-      <c r="E270" s="34"/>
-      <c r="F270" s="34"/>
-      <c r="G270" s="34"/>
-      <c r="H270" s="34"/>
-      <c r="I270" s="34"/>
+      <c r="C270" s="31"/>
+      <c r="D270" s="31"/>
+      <c r="E270" s="31"/>
+      <c r="F270" s="31"/>
+      <c r="G270" s="31"/>
+      <c r="H270" s="31"/>
+      <c r="I270" s="31"/>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B271" s="34"/>
-      <c r="C271" s="34"/>
-      <c r="D271" s="34"/>
-      <c r="E271" s="34"/>
-      <c r="F271" s="34"/>
-      <c r="G271" s="34"/>
-      <c r="H271" s="34"/>
-      <c r="I271" s="34"/>
+      <c r="B271" s="31"/>
+      <c r="C271" s="31"/>
+      <c r="D271" s="31"/>
+      <c r="E271" s="31"/>
+      <c r="F271" s="31"/>
+      <c r="G271" s="31"/>
+      <c r="H271" s="31"/>
+      <c r="I271" s="31"/>
     </row>
     <row r="273" spans="1:9" ht="20" x14ac:dyDescent="0.4">
       <c r="B273"/>
@@ -7006,56 +7006,56 @@
       <c r="A275" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B275" s="34" t="s">
+      <c r="B275" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C275" s="34"/>
-      <c r="D275" s="34"/>
-      <c r="E275" s="34"/>
-      <c r="F275" s="34"/>
-      <c r="G275" s="34"/>
-      <c r="H275" s="34"/>
-      <c r="I275" s="34"/>
+      <c r="C275" s="31"/>
+      <c r="D275" s="31"/>
+      <c r="E275" s="31"/>
+      <c r="F275" s="31"/>
+      <c r="G275" s="31"/>
+      <c r="H275" s="31"/>
+      <c r="I275" s="31"/>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B276" s="34"/>
-      <c r="C276" s="34"/>
-      <c r="D276" s="34"/>
-      <c r="E276" s="34"/>
-      <c r="F276" s="34"/>
-      <c r="G276" s="34"/>
-      <c r="H276" s="34"/>
-      <c r="I276" s="34"/>
+      <c r="B276" s="31"/>
+      <c r="C276" s="31"/>
+      <c r="D276" s="31"/>
+      <c r="E276" s="31"/>
+      <c r="F276" s="31"/>
+      <c r="G276" s="31"/>
+      <c r="H276" s="31"/>
+      <c r="I276" s="31"/>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B277" s="34"/>
-      <c r="C277" s="34"/>
-      <c r="D277" s="34"/>
-      <c r="E277" s="34"/>
-      <c r="F277" s="34"/>
-      <c r="G277" s="34"/>
-      <c r="H277" s="34"/>
-      <c r="I277" s="34"/>
+      <c r="B277" s="31"/>
+      <c r="C277" s="31"/>
+      <c r="D277" s="31"/>
+      <c r="E277" s="31"/>
+      <c r="F277" s="31"/>
+      <c r="G277" s="31"/>
+      <c r="H277" s="31"/>
+      <c r="I277" s="31"/>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B278" s="34"/>
-      <c r="C278" s="34"/>
-      <c r="D278" s="34"/>
-      <c r="E278" s="34"/>
-      <c r="F278" s="34"/>
-      <c r="G278" s="34"/>
-      <c r="H278" s="34"/>
-      <c r="I278" s="34"/>
+      <c r="B278" s="31"/>
+      <c r="C278" s="31"/>
+      <c r="D278" s="31"/>
+      <c r="E278" s="31"/>
+      <c r="F278" s="31"/>
+      <c r="G278" s="31"/>
+      <c r="H278" s="31"/>
+      <c r="I278" s="31"/>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H286" s="34" t="s">
+      <c r="H286" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="I286" s="34"/>
+      <c r="I286" s="31"/>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H287" s="34"/>
-      <c r="I287" s="34"/>
+      <c r="H287" s="31"/>
+      <c r="I287" s="31"/>
     </row>
     <row r="289" spans="1:9" ht="20" x14ac:dyDescent="0.4">
       <c r="H289"/>
@@ -7064,27 +7064,27 @@
       <c r="A291" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="B291" s="34" t="s">
+      <c r="B291" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="C291" s="34"/>
-      <c r="D291" s="34"/>
-      <c r="E291" s="34"/>
-      <c r="F291" s="34"/>
-      <c r="G291" s="34"/>
-      <c r="H291" s="34"/>
-      <c r="I291" s="34"/>
+      <c r="C291" s="31"/>
+      <c r="D291" s="31"/>
+      <c r="E291" s="31"/>
+      <c r="F291" s="31"/>
+      <c r="G291" s="31"/>
+      <c r="H291" s="31"/>
+      <c r="I291" s="31"/>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A292" s="30"/>
-      <c r="B292" s="34"/>
-      <c r="C292" s="34"/>
-      <c r="D292" s="34"/>
-      <c r="E292" s="34"/>
-      <c r="F292" s="34"/>
-      <c r="G292" s="34"/>
-      <c r="H292" s="34"/>
-      <c r="I292" s="34"/>
+      <c r="B292" s="31"/>
+      <c r="C292" s="31"/>
+      <c r="D292" s="31"/>
+      <c r="E292" s="31"/>
+      <c r="F292" s="31"/>
+      <c r="G292" s="31"/>
+      <c r="H292" s="31"/>
+      <c r="I292" s="31"/>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A294" s="6">
@@ -7101,26 +7101,26 @@
       <c r="A313" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B313" s="34" t="s">
+      <c r="B313" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C313" s="34"/>
-      <c r="D313" s="34"/>
-      <c r="E313" s="34"/>
-      <c r="F313" s="34"/>
-      <c r="G313" s="34"/>
-      <c r="H313" s="34"/>
-      <c r="I313" s="34"/>
+      <c r="C313" s="31"/>
+      <c r="D313" s="31"/>
+      <c r="E313" s="31"/>
+      <c r="F313" s="31"/>
+      <c r="G313" s="31"/>
+      <c r="H313" s="31"/>
+      <c r="I313" s="31"/>
     </row>
     <row r="314" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B314" s="34"/>
-      <c r="C314" s="34"/>
-      <c r="D314" s="34"/>
-      <c r="E314" s="34"/>
-      <c r="F314" s="34"/>
-      <c r="G314" s="34"/>
-      <c r="H314" s="34"/>
-      <c r="I314" s="34"/>
+      <c r="B314" s="31"/>
+      <c r="C314" s="31"/>
+      <c r="D314" s="31"/>
+      <c r="E314" s="31"/>
+      <c r="F314" s="31"/>
+      <c r="G314" s="31"/>
+      <c r="H314" s="31"/>
+      <c r="I314" s="31"/>
     </row>
     <row r="315" spans="1:9" ht="20" x14ac:dyDescent="0.4">
       <c r="B315"/>
@@ -7134,88 +7134,88 @@
       <c r="A326" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B326" s="33" t="s">
+      <c r="B326" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C326" s="33"/>
-      <c r="D326" s="33"/>
-      <c r="E326" s="33"/>
-      <c r="F326" s="33"/>
-      <c r="G326" s="33"/>
-      <c r="H326" s="33"/>
-      <c r="I326" s="33"/>
+      <c r="C326" s="32"/>
+      <c r="D326" s="32"/>
+      <c r="E326" s="32"/>
+      <c r="F326" s="32"/>
+      <c r="G326" s="32"/>
+      <c r="H326" s="32"/>
+      <c r="I326" s="32"/>
     </row>
     <row r="327" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B327" s="33"/>
-      <c r="C327" s="33"/>
-      <c r="D327" s="33"/>
-      <c r="E327" s="33"/>
-      <c r="F327" s="33"/>
-      <c r="G327" s="33"/>
-      <c r="H327" s="33"/>
-      <c r="I327" s="33"/>
+      <c r="B327" s="32"/>
+      <c r="C327" s="32"/>
+      <c r="D327" s="32"/>
+      <c r="E327" s="32"/>
+      <c r="F327" s="32"/>
+      <c r="G327" s="32"/>
+      <c r="H327" s="32"/>
+      <c r="I327" s="32"/>
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B328" s="33"/>
-      <c r="C328" s="33"/>
-      <c r="D328" s="33"/>
-      <c r="E328" s="33"/>
-      <c r="F328" s="33"/>
-      <c r="G328" s="33"/>
-      <c r="H328" s="33"/>
-      <c r="I328" s="33"/>
+      <c r="B328" s="32"/>
+      <c r="C328" s="32"/>
+      <c r="D328" s="32"/>
+      <c r="E328" s="32"/>
+      <c r="F328" s="32"/>
+      <c r="G328" s="32"/>
+      <c r="H328" s="32"/>
+      <c r="I328" s="32"/>
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B329" s="33"/>
-      <c r="C329" s="33"/>
-      <c r="D329" s="33"/>
-      <c r="E329" s="33"/>
-      <c r="F329" s="33"/>
-      <c r="G329" s="33"/>
-      <c r="H329" s="33"/>
-      <c r="I329" s="33"/>
+      <c r="B329" s="32"/>
+      <c r="C329" s="32"/>
+      <c r="D329" s="32"/>
+      <c r="E329" s="32"/>
+      <c r="F329" s="32"/>
+      <c r="G329" s="32"/>
+      <c r="H329" s="32"/>
+      <c r="I329" s="32"/>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G330" s="31" t="s">
+      <c r="G330" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="H330" s="31"/>
+      <c r="H330" s="44"/>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G331" s="31"/>
-      <c r="H331" s="31"/>
+      <c r="G331" s="44"/>
+      <c r="H331" s="44"/>
     </row>
     <row r="332" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G332" s="31"/>
-      <c r="H332" s="31"/>
+      <c r="G332" s="44"/>
+      <c r="H332" s="44"/>
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G333" s="31"/>
-      <c r="H333" s="31"/>
+      <c r="G333" s="44"/>
+      <c r="H333" s="44"/>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G334" s="31"/>
-      <c r="H334" s="31"/>
+      <c r="G334" s="44"/>
+      <c r="H334" s="44"/>
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G335" s="31"/>
-      <c r="H335" s="31"/>
+      <c r="G335" s="44"/>
+      <c r="H335" s="44"/>
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G336" s="31"/>
-      <c r="H336" s="31"/>
+      <c r="G336" s="44"/>
+      <c r="H336" s="44"/>
     </row>
     <row r="337" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G337" s="31"/>
-      <c r="H337" s="31"/>
+      <c r="G337" s="44"/>
+      <c r="H337" s="44"/>
     </row>
     <row r="338" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G338" s="31"/>
-      <c r="H338" s="31"/>
+      <c r="G338" s="44"/>
+      <c r="H338" s="44"/>
     </row>
     <row r="339" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G339" s="31"/>
-      <c r="H339" s="31"/>
+      <c r="G339" s="44"/>
+      <c r="H339" s="44"/>
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B341" s="2" t="s">
@@ -7229,67 +7229,67 @@
       <c r="A351" s="6">
         <v>14</v>
       </c>
-      <c r="B351" s="44" t="s">
+      <c r="B351" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C351" s="44"/>
-      <c r="D351" s="44"/>
+      <c r="C351" s="33"/>
+      <c r="D351" s="33"/>
     </row>
     <row r="352" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A352" s="7"/>
-      <c r="B352" s="34" t="s">
+      <c r="B352" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="C352" s="34"/>
-      <c r="D352" s="34"/>
-      <c r="E352" s="34"/>
-      <c r="F352" s="34"/>
-      <c r="G352" s="34"/>
-      <c r="H352" s="34"/>
-      <c r="I352" s="34"/>
+      <c r="C352" s="31"/>
+      <c r="D352" s="31"/>
+      <c r="E352" s="31"/>
+      <c r="F352" s="31"/>
+      <c r="G352" s="31"/>
+      <c r="H352" s="31"/>
+      <c r="I352" s="31"/>
     </row>
     <row r="353" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A353" s="7"/>
-      <c r="B353" s="34"/>
-      <c r="C353" s="34"/>
-      <c r="D353" s="34"/>
-      <c r="E353" s="34"/>
-      <c r="F353" s="34"/>
-      <c r="G353" s="34"/>
-      <c r="H353" s="34"/>
-      <c r="I353" s="34"/>
+      <c r="B353" s="31"/>
+      <c r="C353" s="31"/>
+      <c r="D353" s="31"/>
+      <c r="E353" s="31"/>
+      <c r="F353" s="31"/>
+      <c r="G353" s="31"/>
+      <c r="H353" s="31"/>
+      <c r="I353" s="31"/>
     </row>
     <row r="355" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B355" s="33" t="s">
+      <c r="B355" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C355" s="33"/>
-      <c r="D355" s="33"/>
-      <c r="E355" s="33"/>
-      <c r="F355" s="33"/>
-      <c r="G355" s="33"/>
-      <c r="H355" s="33"/>
-      <c r="I355" s="33"/>
+      <c r="C355" s="32"/>
+      <c r="D355" s="32"/>
+      <c r="E355" s="32"/>
+      <c r="F355" s="32"/>
+      <c r="G355" s="32"/>
+      <c r="H355" s="32"/>
+      <c r="I355" s="32"/>
     </row>
     <row r="356" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B356" s="33"/>
-      <c r="C356" s="33"/>
-      <c r="D356" s="33"/>
-      <c r="E356" s="33"/>
-      <c r="F356" s="33"/>
-      <c r="G356" s="33"/>
-      <c r="H356" s="33"/>
-      <c r="I356" s="33"/>
+      <c r="B356" s="32"/>
+      <c r="C356" s="32"/>
+      <c r="D356" s="32"/>
+      <c r="E356" s="32"/>
+      <c r="F356" s="32"/>
+      <c r="G356" s="32"/>
+      <c r="H356" s="32"/>
+      <c r="I356" s="32"/>
     </row>
     <row r="357" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B357" s="33"/>
-      <c r="C357" s="33"/>
-      <c r="D357" s="33"/>
-      <c r="E357" s="33"/>
-      <c r="F357" s="33"/>
-      <c r="G357" s="33"/>
-      <c r="H357" s="33"/>
-      <c r="I357" s="33"/>
+      <c r="B357" s="32"/>
+      <c r="C357" s="32"/>
+      <c r="D357" s="32"/>
+      <c r="E357" s="32"/>
+      <c r="F357" s="32"/>
+      <c r="G357" s="32"/>
+      <c r="H357" s="32"/>
+      <c r="I357" s="32"/>
     </row>
     <row r="358" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B358" s="13"/>
@@ -7302,81 +7302,121 @@
       <c r="I358" s="13"/>
     </row>
     <row r="359" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B359" s="33" t="s">
+      <c r="B359" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C359" s="33"/>
-      <c r="D359" s="33"/>
-      <c r="E359" s="33"/>
-      <c r="F359" s="33"/>
-      <c r="G359" s="33"/>
-      <c r="H359" s="33"/>
-      <c r="I359" s="33"/>
+      <c r="C359" s="32"/>
+      <c r="D359" s="32"/>
+      <c r="E359" s="32"/>
+      <c r="F359" s="32"/>
+      <c r="G359" s="32"/>
+      <c r="H359" s="32"/>
+      <c r="I359" s="32"/>
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B360" s="33"/>
-      <c r="C360" s="33"/>
-      <c r="D360" s="33"/>
-      <c r="E360" s="33"/>
-      <c r="F360" s="33"/>
-      <c r="G360" s="33"/>
-      <c r="H360" s="33"/>
-      <c r="I360" s="33"/>
+      <c r="B360" s="32"/>
+      <c r="C360" s="32"/>
+      <c r="D360" s="32"/>
+      <c r="E360" s="32"/>
+      <c r="F360" s="32"/>
+      <c r="G360" s="32"/>
+      <c r="H360" s="32"/>
+      <c r="I360" s="32"/>
     </row>
     <row r="361" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B361" s="33"/>
-      <c r="C361" s="33"/>
-      <c r="D361" s="33"/>
-      <c r="E361" s="33"/>
-      <c r="F361" s="33"/>
-      <c r="G361" s="33"/>
-      <c r="H361" s="33"/>
-      <c r="I361" s="33"/>
+      <c r="B361" s="32"/>
+      <c r="C361" s="32"/>
+      <c r="D361" s="32"/>
+      <c r="E361" s="32"/>
+      <c r="F361" s="32"/>
+      <c r="G361" s="32"/>
+      <c r="H361" s="32"/>
+      <c r="I361" s="32"/>
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A363" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B363" s="44" t="s">
+      <c r="B363" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C363" s="44"/>
-      <c r="D363" s="44"/>
+      <c r="C363" s="33"/>
+      <c r="D363" s="33"/>
     </row>
     <row r="364" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B364" s="33" t="s">
+      <c r="B364" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C364" s="33"/>
-      <c r="D364" s="33"/>
-      <c r="E364" s="33"/>
-      <c r="F364" s="33"/>
-      <c r="G364" s="33"/>
-      <c r="H364" s="33"/>
-      <c r="I364" s="33"/>
+      <c r="C364" s="32"/>
+      <c r="D364" s="32"/>
+      <c r="E364" s="32"/>
+      <c r="F364" s="32"/>
+      <c r="G364" s="32"/>
+      <c r="H364" s="32"/>
+      <c r="I364" s="32"/>
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B365" s="33"/>
-      <c r="C365" s="33"/>
-      <c r="D365" s="33"/>
-      <c r="E365" s="33"/>
-      <c r="F365" s="33"/>
-      <c r="G365" s="33"/>
-      <c r="H365" s="33"/>
-      <c r="I365" s="33"/>
+      <c r="B365" s="32"/>
+      <c r="C365" s="32"/>
+      <c r="D365" s="32"/>
+      <c r="E365" s="32"/>
+      <c r="F365" s="32"/>
+      <c r="G365" s="32"/>
+      <c r="H365" s="32"/>
+      <c r="I365" s="32"/>
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B366" s="33"/>
-      <c r="C366" s="33"/>
-      <c r="D366" s="33"/>
-      <c r="E366" s="33"/>
-      <c r="F366" s="33"/>
-      <c r="G366" s="33"/>
-      <c r="H366" s="33"/>
-      <c r="I366" s="33"/>
+      <c r="B366" s="32"/>
+      <c r="C366" s="32"/>
+      <c r="D366" s="32"/>
+      <c r="E366" s="32"/>
+      <c r="F366" s="32"/>
+      <c r="G366" s="32"/>
+      <c r="H366" s="32"/>
+      <c r="I366" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="G330:H339"/>
+    <mergeCell ref="G16:I24"/>
+    <mergeCell ref="C74:I77"/>
+    <mergeCell ref="B206:I210"/>
+    <mergeCell ref="B291:I292"/>
+    <mergeCell ref="B99:I104"/>
+    <mergeCell ref="B235:I237"/>
+    <mergeCell ref="B240:I240"/>
+    <mergeCell ref="B275:I278"/>
+    <mergeCell ref="H286:I287"/>
+    <mergeCell ref="B192:I193"/>
+    <mergeCell ref="B153:I155"/>
+    <mergeCell ref="B234:I234"/>
+    <mergeCell ref="B143:I144"/>
+    <mergeCell ref="H146:I149"/>
+    <mergeCell ref="B214:C220"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B56:H59"/>
+    <mergeCell ref="B135:I137"/>
+    <mergeCell ref="H2:I8"/>
+    <mergeCell ref="H9:I11"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="G12:I15"/>
+    <mergeCell ref="C79:I82"/>
+    <mergeCell ref="H118:I119"/>
+    <mergeCell ref="H121:I122"/>
+    <mergeCell ref="B68:B72"/>
+    <mergeCell ref="C68:D72"/>
+    <mergeCell ref="A3:F9"/>
+    <mergeCell ref="H63:I66"/>
+    <mergeCell ref="E68:G72"/>
+    <mergeCell ref="G115:I116"/>
+    <mergeCell ref="B203:I204"/>
+    <mergeCell ref="B86:I89"/>
+    <mergeCell ref="B94:I96"/>
+    <mergeCell ref="F157:I160"/>
+    <mergeCell ref="B98:I98"/>
+    <mergeCell ref="B140:I141"/>
+    <mergeCell ref="B166:I166"/>
+    <mergeCell ref="B175:I176"/>
     <mergeCell ref="B266:I268"/>
     <mergeCell ref="B270:I271"/>
     <mergeCell ref="B91:I92"/>
@@ -7393,46 +7433,6 @@
     <mergeCell ref="B241:I244"/>
     <mergeCell ref="B351:D351"/>
     <mergeCell ref="B179:I180"/>
-    <mergeCell ref="B203:I204"/>
-    <mergeCell ref="B86:I89"/>
-    <mergeCell ref="B94:I96"/>
-    <mergeCell ref="F157:I160"/>
-    <mergeCell ref="B98:I98"/>
-    <mergeCell ref="B140:I141"/>
-    <mergeCell ref="B166:I166"/>
-    <mergeCell ref="B175:I176"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B56:H59"/>
-    <mergeCell ref="B135:I137"/>
-    <mergeCell ref="H2:I8"/>
-    <mergeCell ref="H9:I11"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="G12:I15"/>
-    <mergeCell ref="C79:I82"/>
-    <mergeCell ref="H118:I119"/>
-    <mergeCell ref="H121:I122"/>
-    <mergeCell ref="B68:B72"/>
-    <mergeCell ref="C68:D72"/>
-    <mergeCell ref="A3:F9"/>
-    <mergeCell ref="H63:I66"/>
-    <mergeCell ref="E68:G72"/>
-    <mergeCell ref="G115:I116"/>
-    <mergeCell ref="G330:H339"/>
-    <mergeCell ref="G16:I24"/>
-    <mergeCell ref="C74:I77"/>
-    <mergeCell ref="B206:I210"/>
-    <mergeCell ref="B291:I292"/>
-    <mergeCell ref="B99:I104"/>
-    <mergeCell ref="B235:I237"/>
-    <mergeCell ref="B240:I240"/>
-    <mergeCell ref="B275:I278"/>
-    <mergeCell ref="H286:I287"/>
-    <mergeCell ref="B192:I193"/>
-    <mergeCell ref="B153:I155"/>
-    <mergeCell ref="B234:I234"/>
-    <mergeCell ref="B143:I144"/>
-    <mergeCell ref="H146:I149"/>
-    <mergeCell ref="B214:C220"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7496,8 +7496,8 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="45"/>
@@ -7507,8 +7507,8 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="45"/>
@@ -7721,7 +7721,7 @@
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="32" t="s">
         <v>82</v>
       </c>
       <c r="B24" s="2"/>
@@ -7734,7 +7734,7 @@
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A25" s="33"/>
+      <c r="A25" s="32"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -7744,7 +7744,7 @@
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A26" s="33"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -7755,7 +7755,7 @@
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A27" s="33"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -7766,7 +7766,7 @@
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A28" s="33"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -7777,7 +7777,7 @@
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="33"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>

</xml_diff>

<commit_message>
working on the diff between level 1 and level 2 review SOP
as well as the report
</commit_message>
<xml_diff>
--- a/hosted_files/QREST/QREST-Level 2 Data Review.xlsx
+++ b/hosted_files/QREST/QREST-Level 2 Data Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melinda\Documents\GitHub\tamscenter.github.io\hosted_files\QREST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BF1B752-6DBA-4F6D-9A62-8D5EB8FCC9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4148AA-2053-4D22-81B7-6C6B641B0252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-1850" windowWidth="19420" windowHeight="10560" xr2:uid="{7715871D-8683-4309-BD27-314EA3A9CF8F}"/>
   </bookViews>
@@ -5527,8 +5527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CD1C20-C544-4641-A5D7-3C5C166E6123}">
   <dimension ref="A1:I366"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A265" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="J362" sqref="J362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>